<commit_message>
Na classe Agenda foi criado o metodo para inserir o cliente na planilha do Excel e o metodo para procurar a linha vazia antes da insercao. Modificado a classe Program para instanciar a Agenda e chamar o metodo para salvar o cliente na planilha do Excel
</commit_message>
<xml_diff>
--- a/AGENDAKATIA.xlsx
+++ b/AGENDAKATIA.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\zEstudo\ProgramasTeste\TesteAMexendoComTabelaExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\zWorkFolder\PreencherAgendaExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Contatos01" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Contatos01!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Contatos01!$A$1:$N$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
   <si>
     <t>NOME</t>
   </si>
@@ -44,6 +44,9 @@
     <t>EMAIL</t>
   </si>
   <si>
+    <t>TELEFONE</t>
+  </si>
+  <si>
     <t>CONVÊNIO EMPRESA</t>
   </si>
   <si>
@@ -59,21 +62,18 @@
     <t>COMPLEMENTO</t>
   </si>
   <si>
+    <t>BAIRRO</t>
+  </si>
+  <si>
+    <t>CIDADE</t>
+  </si>
+  <si>
+    <t>ESTADO</t>
+  </si>
+  <si>
     <t>CEP</t>
   </si>
   <si>
-    <t>BAIRRO</t>
-  </si>
-  <si>
-    <t>CIDADE</t>
-  </si>
-  <si>
-    <t>ESTADO</t>
-  </si>
-  <si>
-    <t>TELEFONE</t>
-  </si>
-  <si>
     <t>GABRIEL DANTAS COSTA</t>
   </si>
   <si>
@@ -95,9 +95,6 @@
     <t>CASA</t>
   </si>
   <si>
-    <t>02872030</t>
-  </si>
-  <si>
     <t>JARDIM CECY</t>
   </si>
   <si>
@@ -128,9 +125,6 @@
     <t>APTO 61A</t>
   </si>
   <si>
-    <t>02415001</t>
-  </si>
-  <si>
     <t>PARQUE MANDAQUI</t>
   </si>
   <si>
@@ -146,16 +140,67 @@
     <t>RUA HENRIQUE VIII</t>
   </si>
   <si>
-    <t>07845080</t>
-  </si>
-  <si>
     <t>JARDIM DOS REIS</t>
+  </si>
+  <si>
+    <t>GUILERME DE SOUZA ANTUNES</t>
+  </si>
+  <si>
+    <t>rosanacsantunes@yahoo.com.br</t>
+  </si>
+  <si>
+    <t>BRADESCO</t>
+  </si>
+  <si>
+    <t>RESE NACIONAL</t>
+  </si>
+  <si>
+    <t>ESTRADA DO SABÃO</t>
+  </si>
+  <si>
+    <t>JARDIM MARISTELA</t>
+  </si>
+  <si>
+    <t>GUILHERME DE SOUZA CAMPOS</t>
+  </si>
+  <si>
+    <t>CAASP</t>
+  </si>
+  <si>
+    <t>CAMPANHA DA BOA VISAO</t>
+  </si>
+  <si>
+    <t>RUA PEDRO</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>VILA ALBERTINA</t>
+  </si>
+  <si>
+    <t>02806-000</t>
+  </si>
+  <si>
+    <t>07845-080</t>
+  </si>
+  <si>
+    <t>02415-001</t>
+  </si>
+  <si>
+    <t>02872-030</t>
+  </si>
+  <si>
+    <t>guaracampus@yahoo.com.br</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="00000\-000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -194,7 +239,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -215,6 +260,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -501,26 +549,26 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="13" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="27.44140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" style="3" customWidth="1"/>
-    <col min="10" max="10" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9" style="7" customWidth="1"/>
-    <col min="12" max="12" width="18.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.21875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.21875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="12.21875" style="2" customWidth="1"/>
     <col min="14" max="14" width="7.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.6640625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="11.88671875" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -554,7 +602,7 @@
       <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
@@ -566,7 +614,7 @@
       <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="7" t="s">
         <v>14</v>
       </c>
     </row>
@@ -587,43 +635,43 @@
       <c r="E2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="2">
+        <v>11942942557</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="3">
+      <c r="J2" s="3">
         <v>225</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="L2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O2" s="2">
-        <v>11942942557</v>
+      <c r="O2" s="8" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="C3" s="4">
         <v>20351</v>
@@ -633,42 +681,42 @@
         <v>64</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1129527686</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="I3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="J3" s="3">
+        <v>881</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="3">
-        <v>881</v>
-      </c>
-      <c r="J3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="M3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="N3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O3" s="2">
-        <v>1129527686</v>
+      <c r="O3" s="8" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>16</v>
@@ -681,50 +729,152 @@
         <v>37</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="2">
+        <v>11988679854</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="2" t="s">
+      <c r="J4" s="3">
+        <v>301</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="M4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I4" s="3">
-        <v>301</v>
-      </c>
-      <c r="J4" s="2" t="s">
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="4">
+        <v>34283</v>
+      </c>
+      <c r="D5" s="6">
+        <v>26</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1138243462</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="3">
+        <v>1395</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="M4" s="2" t="s">
+      <c r="L5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="N4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O4" s="2">
-        <v>11988679854</v>
-      </c>
+      <c r="O5" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="4">
+        <v>36559</v>
+      </c>
+      <c r="D6" s="6">
+        <v>20</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1122032680</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J6" s="3">
+        <v>843</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O6" s="8">
+        <v>2371000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O7"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G8"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="G13"/>
+      <c r="H13"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O1"/>
+  <autoFilter ref="A1:N1"/>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
     <hyperlink ref="E3" r:id="rId2"/>
     <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>